<commit_message>
Addition of manage defaults and other scripts
</commit_message>
<xml_diff>
--- a/testdata/FCfiles/qa/ManageLocations/ManageLocations.xlsx
+++ b/testdata/FCfiles/qa/ManageLocations/ManageLocations.xlsx
@@ -1,17 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\qualitesoft\testdata\FCfiles\qa\ManageLocations\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E394973-8147-46FB-806A-7F8F81D05376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="449"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="449" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Input" sheetId="1" r:id="rId1"/>
+    <sheet name="ManageLocation" sheetId="1" r:id="rId1"/>
+    <sheet name="Input" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="87">
   <si>
     <t>CompanyName</t>
   </si>
@@ -139,13 +146,154 @@
   </si>
   <si>
     <t>a1@gmail.com</t>
+  </si>
+  <si>
+    <t>shipmentType</t>
+  </si>
+  <si>
+    <t>pickUpDate</t>
+  </si>
+  <si>
+    <t>serviceLevel</t>
+  </si>
+  <si>
+    <t>orderReferenceID</t>
+  </si>
+  <si>
+    <t>pickUpZip</t>
+  </si>
+  <si>
+    <t>pickUpLocationName</t>
+  </si>
+  <si>
+    <t>pickUpType</t>
+  </si>
+  <si>
+    <t>dropOffZip</t>
+  </si>
+  <si>
+    <t>dropOffLocationName</t>
+  </si>
+  <si>
+    <t>dropOffType</t>
+  </si>
+  <si>
+    <t>Insurance</t>
+  </si>
+  <si>
+    <t>packageType</t>
+  </si>
+  <si>
+    <t>packageType2</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>DimensionL</t>
+  </si>
+  <si>
+    <t>DimensionW</t>
+  </si>
+  <si>
+    <t>DimensionH</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>DeclaredValue</t>
+  </si>
+  <si>
+    <t>Cartons</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Carrier</t>
+  </si>
+  <si>
+    <t>OrderId</t>
+  </si>
+  <si>
+    <t>CloneOrderId</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Tracking#</t>
+  </si>
+  <si>
+    <t>WayBill</t>
+  </si>
+  <si>
+    <t>PalletType1</t>
+  </si>
+  <si>
+    <t>PalletType2</t>
+  </si>
+  <si>
+    <t>CartoonQuantity</t>
+  </si>
+  <si>
+    <t>TotalPalletCount</t>
+  </si>
+  <si>
+    <t>PalletWeight</t>
+  </si>
+  <si>
+    <t>TotalNumberOfLabels</t>
+  </si>
+  <si>
+    <t>BOLCount</t>
+  </si>
+  <si>
+    <t>Less Than Truckload</t>
+  </si>
+  <si>
+    <t>09-11-2022</t>
+  </si>
+  <si>
+    <t>Curbside (Liftgate)</t>
+  </si>
+  <si>
+    <t>TestOrder1</t>
+  </si>
+  <si>
+    <t>Non-Palletized</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>600</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Ceva</t>
+  </si>
+  <si>
+    <t>Amazon FBA Warehouse</t>
+  </si>
+  <si>
+    <t>Order Administrator</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,21 +320,49 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -197,15 +373,35 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="18" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -479,299 +675,633 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="10.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="14.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="13.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="19" width="10.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="19.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="14.109375" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="13.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="19" width="10.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="12.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="19.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="16384" width="9.109375" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" t="s">
         <v>19</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="N3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="6" t="s">
+      <c r="F4" s="2"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="1"/>
+      <c r="J4" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" t="s">
         <v>19</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="M4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="N4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:14" customFormat="1">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="K5" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="L5" t="s">
         <v>19</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="M5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="N5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:14" customFormat="1">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="6" t="s">
+      <c r="F6" s="2"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="1"/>
+      <c r="J6" t="s">
         <v>36</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="K6" t="s">
         <v>36</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="L6" t="s">
         <v>37</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="M6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="N6" s="7" t="s">
+      <c r="N6" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="1"/>
+      <c r="J7" t="s">
+        <v>86</v>
+      </c>
+      <c r="K7" t="s">
+        <v>36</v>
+      </c>
+      <c r="L7" t="s">
+        <v>37</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N7" s="3" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="N6" r:id="rId1"/>
+    <hyperlink ref="N6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="N7" r:id="rId2" xr:uid="{3AE98C7E-C6BF-4155-8944-812E7E337705}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FFF0322-742A-4FCA-B00A-3DE390CABF4C}">
+  <dimension ref="A1:AH3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="S1" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="T1" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="U1" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="V1" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="W1" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="X1" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y1" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z1" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA1" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB1" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC1" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD1" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE1" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF1" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG1" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="AH1" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="M2" s="4"/>
+      <c r="N2" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="U2" s="6">
+        <v>10</v>
+      </c>
+      <c r="V2" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="6"/>
+      <c r="AB2" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC2" s="4"/>
+      <c r="AD2" s="4"/>
+      <c r="AE2" s="4"/>
+      <c r="AF2" s="4"/>
+      <c r="AG2" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH2" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="5"/>
+      <c r="J3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="M3" s="4"/>
+      <c r="N3" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="U3" s="6">
+        <v>10</v>
+      </c>
+      <c r="V3" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="6"/>
+      <c r="AA3" s="6"/>
+      <c r="AB3" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC3" s="4"/>
+      <c r="AD3" s="4"/>
+      <c r="AE3" s="4"/>
+      <c r="AF3" s="4"/>
+      <c r="AG3" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH3" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>